<commit_message>
Add files via upload 886ed49ce9f3fed0f5796af29e39e97971e99b1a
</commit_message>
<xml_diff>
--- a/260-location-status/ig/StructureDefinition-ror-organization.xlsx
+++ b/260-location-status/ig/StructureDefinition-ror-organization.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-05-02T15:56:22+00:00</t>
+    <t>2024-05-02T16:52:08+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1316,7 +1316,7 @@
   <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
   &lt;coding&gt;
-    &lt;system value="https://mos.esante.gouv.fr/NOS/TRE_R345-TypeIdentifiantAutre/FHIR/TRE-R345-TypeIdentifiantAutre"/&gt;
+    &lt;system value="https://mos.esante.gouv.fr/NOS/TRE_R345-TypeIdentifiantAutre/FHIR/TRE_R345-TypeIdentifiantAutre"/&gt;
     &lt;code value="42"/&gt;
   &lt;/coding&gt;
 &lt;/valueCodeableConcept&gt;</t>

</xml_diff>